<commit_message>
Modificar función de carga para borrar datos anteriores al subir nuevo archivo
</commit_message>
<xml_diff>
--- a/front/CONSOLIDADO EMBARGOS.xlsx
+++ b/front/CONSOLIDADO EMBARGOS.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="2" documentId="8_{79625243-C36A-46DD-B172-BCA44B354C4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{42B3B527-C9E0-43F2-B202-1828094A91CB}"/>
   <bookViews>
-    <workbookView xWindow="-113" yWindow="-113" windowWidth="21262" windowHeight="12647" xr2:uid="{5DC27DB5-4B88-4F71-A635-A8578603720B}"/>
+    <workbookView xWindow="2554" yWindow="2554" windowWidth="15778" windowHeight="9016" xr2:uid="{5DC27DB5-4B88-4F71-A635-A8578603720B}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -600,7 +600,7 @@
   <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="O7" sqref="O7"/>
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>

</xml_diff>